<commit_message>
preparing feature-specific data in wide format
</commit_message>
<xml_diff>
--- a/DataRaw/DeidentifiedRaw.xlsx
+++ b/DataRaw/DeidentifiedRaw.xlsx
@@ -5,7 +5,7 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3c2d16a148962151/Desktop/BIOSTAT/Thesis/Journal/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3c2d16a148962151/Desktop/BIOSTAT/Thesis/Journal/DataRaw/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="42" documentId="8_{B24AA457-39B2-4231-999B-129B4C0C87CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3464FD1A-0C14-45B1-B420-C429BB2458F9}"/>
@@ -2479,7 +2479,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -2555,7 +2555,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -2626,7 +2626,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -2638,10 +2638,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -30907,7 +30903,7 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="B158:B162">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="notEqual">
       <formula>B158</formula>
     </cfRule>
   </conditionalFormatting>
@@ -30932,7 +30928,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>BC51:BE51 F3:BE33 F34:BF50 F51:BB52 BD52:BE52 O53:BE53 F53:M55 O54:BB54 BD54:BE57 N55:BB55 L56:BB56 F56:K57 M57:O57 Q57:BB57 F58:M58 O58:BE58 F59:BE59 M60:BE64 F60:L65 N65:AU65 AW65:BE65 M66 O66:BB66 BD66:BE66 F66:K72 L67:BE67 R68:BE68 L68:P69 Q69:AY69 BA69:BE69 L70:M70 O70:BE70 BE71 M71:BB72 BD72:BE75 F73:BB73 N74:BB74 F74:L80 O75:BB75 M75:M80 N76:BF76 AT77:BE77 N77:AR80 AS78:BE80 F81:AU81 AY81:BC81 BE81 M82:O82 Q82:AT82 AV82:AX82 AZ82:BB82 BD82:BF82 F82:K93 L83:BF83 M84:AO84 AQ84:BF84 BD85:BF85 L85:BB86 BC86:BF86 N87:BB87 BD87:BE89 L87:L93 O88:BB88 BF88:BF89 M88:M93 O89:P89 R89:AU89 AW89 AY89:BB89 N90:BE92 BF91 N93:AQ93 AS93:AU93 AW93 AY93:BF93 F94:BF94 R95:BF95 F95:P96 Q96:AU96 AW96 AY96:BF96 F97:M97 O97:BF97 M98:BB98 BD98:BF99 F98:K107 L99:BB99 L100:O100 Q100:BF100 O101:BF101 L101:M102 N102:AY102 BA102:BF102 M103:O103 R103:BF103 AW104 AZ104:BF104 L104:AU105 AV105:BF105 M106:N106 P106:BF106 M107 O107:BE107 F108:L108 O108:AW108 AY108:BF108 AY109:AZ109 BB109:BF109 F109:AW113 AX110:BB111 BD110:BF111 AY112:BE112 AX113:BE113 M114:BE114 F114:K125 BD115:BE115 L115:BB116 BC116:BF116 N117:AR117 AT117:AU117 AW117:AX117 BB117:BF117 L118:AY118 BA118:BF118 N119:AS119 AU119:BF119 L119:L120 M120:BB120 BD120:BF121 M121:P121 R121:AY121 BA121:BB121 AW122:BF122 L122:AU125 AV123:BF125 F126:AO126 AQ126:AU126 AW126:AX126 AZ126:BF126 F127:BF127 F128:BB128 BD128:BF128 F129:AS129 AU129:BE129 F130:BD130 F131:BC131 BE131:BF131 F132:BB132 BD132:BE132 R133:AU133 AW133:BC133 BE133 F133:P134 Q134:BF134 F135:O135 Q135:AU135 AW135:BB135 BD135:BF135 O136:BF136 F136:M141 BD137:BF137 N137:BB138 BC138:BF138 N139:AW139 AY139:BE139 R140:BB140 BD140:BF140 N140:P141 Q141:BF141 M142 O142:AU142 AW142 AY142:BB142 BD142:BF142 F142:K160 P143:AX143 AZ143:BF143 L143:N155 AW144:AX144 AZ144:BE144 O144:AU150 AV145:BF146 BD147:BF148 AV147:BB150 BC149:BF149 BD150 AS151:AU151 AW151:BF151 O151:AQ155 AR152:BE154 BF153:BF154 AR155:AU155 BD155:BF155 AW155:BB156 L156 N156:AU156 BD156:BE156 M157:N157 P157:BE157 L158:AU158 AW158 AZ158:BE158 M159:BE159 L160:AW160 AY160:BE160 F161:M162 O161:O162 Q161:AW162 AY161:BB162 BD161:BF162 N162 P162 AX162 BC162</xm:sqref>
+          <xm:sqref>F3:BE33 F34:BF50 BC51:BE51 F51:BB52 BD52:BE52 O53:BE53 F53:M55 O54:BB54 BD54:BE57 N55:BB55 L56:BB56 F56:K57 M57:O57 Q57:BB57 F58:M58 O58:BE58 F59:BE59 M60:BE64 F60:L65 N65:AU65 AW65:BE65 M66 O66:BB66 BD66:BE66 F66:K72 L67:BE67 R68:BE68 L68:P69 Q69:AY69 BA69:BE69 L70:M70 O70:BE70 BE71 M71:BB72 BD72:BE75 F73:BB73 N74:BB74 F74:L80 O75:BB75 M75:M80 N76:BF76 AT77:BE77 N77:AR80 AS78:BE80 F81:AU81 AY81:BC81 BE81 M82:O82 Q82:AT82 AV82:AX82 AZ82:BB82 BD82:BF82 F82:K93 L83:BF83 M84:AO84 AQ84:BF84 BD85:BF85 L85:BB86 BC86:BF86 N87:BB87 BD87:BE89 L87:L93 O88:BB88 BF88:BF89 M88:M93 O89:P89 R89:AU89 AW89 AY89:BB89 N90:BE92 BF91 N93:AQ93 AS93:AU93 AW93 AY93:BF93 F94:BF94 R95:BF95 F95:P96 Q96:AU96 AW96 AY96:BF96 F97:M97 O97:BF97 M98:BB98 BD98:BF99 F98:K107 L99:BB99 L100:O100 Q100:BF100 O101:BF101 L101:M102 N102:AY102 BA102:BF102 M103:O103 R103:BF103 AW104 AZ104:BF104 L104:AU105 AV105:BF105 M106:N106 P106:BF106 M107 O107:BE107 F108:L108 O108:AW108 AY108:BF108 AY109:AZ109 BB109:BF109 F109:AW113 AX110:BB111 BD110:BF111 AY112:BE112 AX113:BE113 M114:BE114 F114:K125 BD115:BE115 L115:BB116 BC116:BF116 N117:AR117 AT117:AU117 AW117:AX117 BB117:BF117 L118:AY118 BA118:BF118 N119:AS119 AU119:BF119 L119:L120 M120:BB120 BD120:BF121 M121:P121 R121:AY121 BA121:BB121 AW122:BF122 L122:AU125 AV123:BF125 F126:AO126 AQ126:AU126 AW126:AX126 AZ126:BF126 F127:BF127 F128:BB128 BD128:BF128 F129:AS129 AU129:BE129 F130:BD130 F131:BC131 BE131:BF131 F132:BB132 BD132:BE132 R133:AU133 AW133:BC133 BE133 F133:P134 Q134:BF134 F135:O135 Q135:AU135 AW135:BB135 BD135:BF135 O136:BF136 F136:M141 BD137:BF137 N137:BB138 BC138:BF138 N139:AW139 AY139:BE139 R140:BB140 BD140:BF140 N140:P141 Q141:BF141 M142 O142:AU142 AW142 AY142:BB142 BD142:BF142 F142:K160 P143:AX143 AZ143:BF143 L143:N155 AW144:AX144 AZ144:BE144 O144:AU150 AV145:BF146 BD147:BF148 AV147:BB150 BC149:BF149 BD150 AS151:AU151 AW151:BF151 O151:AQ155 AR152:BE154 BF153:BF154 AR155:AU155 BD155:BF155 AW155:BB156 L156 N156:AU156 BD156:BE156 M157:N157 P157:BE157 L158:AU158 AW158 AZ158:BE158 M159:BE159 L160:AW160 AY160:BE160 F161:M162 O161:O162 Q161:AW162 AY161:BB162 BD161:BF162 N162 P162 AX162 BC162</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -58912,14 +58908,14 @@
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="L158:AU158 AW158 AZ158:BE158 M159:BE159 L160:AW160 AY160:BE160 O161 Q161:AW161 AY161:BB161 BD161:BF161 N162:BF162 F158:K160 F161:M162">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="notEqual">
-      <formula>F158</formula>
+  <conditionalFormatting sqref="B158:B162">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="notEqual">
+      <formula>B158</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B158:B162">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="notEqual">
-      <formula>B158</formula>
+  <conditionalFormatting sqref="L158:AU158 AW158 AZ158:BE158 F158:K160 M159:BE159 L160:AW160 AY160:BE160 O161 Q161:AW161 AY161:BB161 BD161:BF161 F161:M162 N162:BF162">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="notEqual">
+      <formula>F158</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>